<commit_message>
exploradores ctm all boys
</commit_message>
<xml_diff>
--- a/Lineas.xlsx
+++ b/Lineas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Web Linea Unica</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>Mi Linea Capro</t>
+  </si>
+  <si>
+    <t>Lineas Input</t>
+  </si>
+  <si>
+    <t>Input Mail</t>
   </si>
 </sst>
 </file>
@@ -507,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,6 +1081,22 @@
         <v>1152292615</v>
       </c>
     </row>
+    <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="8">
+        <v>3758649203</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
actualizaciones xml y data provider
</commit_message>
<xml_diff>
--- a/Lineas.xlsx
+++ b/Lineas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Web Linea Unica</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t>Input Mail</t>
+  </si>
+  <si>
+    <t>1162733281</t>
+  </si>
+  <si>
+    <t>3854041917</t>
+  </si>
+  <si>
+    <t>1164473518</t>
   </si>
 </sst>
 </file>
@@ -515,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,8 +700,8 @@
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5">
-        <v>1162733281</v>
+      <c r="B10" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -727,8 +736,8 @@
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="5">
-        <v>1168829219</v>
+      <c r="B12" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -853,8 +862,8 @@
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="5">
-        <v>1164473518</v>
+      <c r="B19" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>

</xml_diff>